<commit_message>
Your update message here
</commit_message>
<xml_diff>
--- a/attendance-files/BM/BM Attendance - B.xlsx
+++ b/attendance-files/BM/BM Attendance - B.xlsx
@@ -5,13 +5,11 @@
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$6:$AA$83</definedName>
-  </definedNames>
+  <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="iHaB1tibNb8ERmxYmgh6dlFhCSs9uEF1GlDBdUk3Uf4="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="+npgQ6uZsrYJrIRFqO2ocs/IDld99E0uIEPAZjtyJns="/>
     </ext>
   </extLst>
 </workbook>
@@ -19212,7 +19210,6 @@
       <c r="V997" s="53"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$6:$AA$83"/>
   <mergeCells count="1">
     <mergeCell ref="G4:Z4"/>
   </mergeCells>

</xml_diff>